<commit_message>
📝 Add a list of functions used in solving problems
</commit_message>
<xml_diff>
--- a/function.xlsx
+++ b/function.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Programming/Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D13AC8-932D-174A-9AA0-DD22A6C92EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA4AA27-0C4A-7B4A-B231-60146ADEC2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="1200" windowWidth="28100" windowHeight="17380" xr2:uid="{2E81AE7D-DA09-DE4E-A788-EC34B3E1715F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{2E81AE7D-DA09-DE4E-A788-EC34B3E1715F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,76 +36,62 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>함수명</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>동작</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>ord()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>하나의 문자를 입력받아 해당 문자의 유니코드 코드 포인트(정수값)를 반환</t>
   </si>
   <si>
     <t>예시</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>print(ord('A'))   # 출력: 65
 print(ord('a'))   # 출력: 97
 print(ord('#'))   # 출력: 35</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>문자열.lower()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>문자열의 모든 대문자를 소문자로 변환후 새로운 문자열을 반환</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>문자열.upper()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>문자열의 모든 소문자를 대문자로 변환후 새로운 문자열을 반환</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>set()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>중복되지 않은 고유한 요소들의 집합을 만드는 데 사용되는 데이터 타입</t>
   </si>
   <si>
     <t>설명</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">반복 가능한 객체(iterable)를 입력으로 받아 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF0E0E0E"/>
-        <rFont val=".SF NS"/>
-      </rPr>
-      <t>중복된 항목을 제거하고, 순서와 상관없이 요소를 저장</t>
-    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>map()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>반복 가능한 객체(iterable)의 모든 요소에 대해 특정 함수를 적용하여 새로운 값을 생성하는 함수</t>
@@ -115,59 +101,136 @@
   </si>
   <si>
     <t>prod()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>리스트나 튜플 등의 반복 가능한(iterable) 객체에 포함된 모든 숫자를 곱한 결과를 반환 (math 모듈)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>from math import prod
 result = prod(iterable)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>bin()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>정수를 이진수 문자열로 변환</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">반환된 문자열은 항상 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 라는 접두어로 시작. 이 접두어는 해당 문자열이 이진수임을 나타내는 표시</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>find()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열 내에서 특정 문자열(substring)을 검색하고, 찾은 위치의 인덱스를 반환</t>
+  </si>
+  <si>
+    <t>반복 가능한 객체(iterable)를 입력으로 받아 중복된 항목을 제거하고, 순서와 상관없이 요소를 저장</t>
+  </si>
+  <si>
+    <t>반환된 문자열은 항상 0b 라는 접두어로 시작. 이 접두어는 해당 문자열이 이진수임을 나타내는 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str.find(sub[, start[, end]])</t>
+  </si>
+  <si>
+    <t>찾고자 하는 문자열이 여러 개 존재하더라도 첫 번째로 발견된 위치의 인덱스만 반환하며, 만약 찾고자 하는 문자열이 없다면 -1을 반환</t>
+  </si>
+  <si>
+    <t>rfind()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오른쪽(문자열의 끝)에서부터 특정 문자열을 검색</t>
+  </si>
+  <si>
+    <t>가장 마지막에 등장하는 위치의 인덱스를 반환. 만약 찾는 문자열이 없으면 -1을 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str.rfind(sub[, start[, end]])</t>
+  </si>
+  <si>
+    <t>rindex()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rfind()와 비슷하게 오른쪽(문자열의 끝)부터 특정 문자열을 검색</t>
+  </si>
+  <si>
+    <t>찾는 문자열이 없을 때 -1을 반환하지 않고, ValueError 예외를 발생</t>
+  </si>
+  <si>
+    <t>str.rindex(sub[, start[, end]])</t>
+  </si>
+  <si>
+    <t>문자열.startswith()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열이 특정 문자열(접두사)로 시작하는지 여부를 확인하고, 결과를 True 또는 False로 반환</t>
+  </si>
+  <si>
+    <t>str.startswith(prefix[, start[, end]])</t>
+  </si>
+  <si>
+    <t>문자열.split()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열을 특정 구분자(기본적으로 공백)를 기준으로 나누어 리스트로 반환</t>
+  </si>
+  <si>
+    <t>str.split(sep=None, maxsplit=-1)</t>
+  </si>
+  <si>
+    <t>리스트.sort()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>리스트의 요소를 정렬하는 메서드</t>
+  </si>
+  <si>
+    <t>리스트를 제자리(in-place)에서 정렬하고, None을 반환</t>
+  </si>
+  <si>
+    <t>list.sort(key=None, reverse=False)</t>
+  </si>
+  <si>
+    <t>sorted()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>리스트나 다른 반복 가능한(iterable) 객체를 정렬하여 새로운 정렬된 리스트를 반환</t>
+  </si>
+  <si>
+    <t>원본 데이터를 변경하지 않고, 정렬된 새로운 리스트를 반환</t>
+  </si>
+  <si>
+    <t>sorted(iterable, key=None, reverse=False)</t>
+  </si>
+  <si>
+    <t>문자열.replace()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>원본 문자열을 수정하지 않고, 대체된 새로운 문자열을 반환</t>
+  </si>
+  <si>
+    <t>문자열에서 특정 부분 문자열을 다른 문자열로 대체</t>
+  </si>
+  <si>
+    <t>str.replace(old, new[, count])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -179,15 +242,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -208,15 +262,18 @@
       <charset val="129"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF0E0E0E"/>
-      <name val=".SF NS"/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="D2Coding"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FF0E0E0E"/>
-      <name val=".SF NS"/>
+      <name val="D2Coding"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -249,24 +306,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -603,19 +657,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC2A21E-DF1E-C041-8210-3C2DEFB4ACD2}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="40" customHeight="1">
@@ -636,10 +691,10 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -647,7 +702,7 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -655,7 +710,7 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -663,48 +718,154 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="40" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="51">
       <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="40" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="40" customHeight="1">
+      <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="40" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="40" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="40" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="40" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="40" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="40" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="40" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add two solutions for Week_3 of programmers (squashed two commits into one: jan 6th and 7th)
</commit_message>
<xml_diff>
--- a/function.xlsx
+++ b/function.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Programming/Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A64AE6-4C12-6A4D-94F5-4F77CA27DD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C4289C-8612-964F-B60A-5B26ACA7F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{2E81AE7D-DA09-DE4E-A788-EC34B3E1715F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>함수명</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -339,6 +339,18 @@
   </si>
   <si>
     <t>string.translate(table)</t>
+  </si>
+  <si>
+    <t>divmod(나누어질 숫자, 나눌 숫자)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나눗셈과 관련된 연산을 한 번에 처리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 함수는 두 숫자를 입력받아 몫과 나머지를 튜플로 반환합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -772,16 +784,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC2A21E-DF1E-C041-8210-3C2DEFB4ACD2}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="120.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1090,6 +1102,17 @@
         <v>83</v>
       </c>
     </row>
+    <row r="26" spans="1:4" ht="40" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>